<commit_message>
exclude CEL given spike
</commit_message>
<xml_diff>
--- a/prod/static_params.xlsx
+++ b/prod/static_params.xlsx
@@ -100,7 +100,7 @@
     <t xml:space="preserve">EXCLUSION_LIST</t>
   </si>
   <si>
-    <t xml:space="preserve">KNC+</t>
+    <t xml:space="preserve">KNC+CEL</t>
   </si>
   <si>
     <t xml:space="preserve">must contain '+'</t>
@@ -583,10 +583,10 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.14"/>
@@ -785,7 +785,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.15"/>
@@ -36798,7 +36798,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.15"/>
@@ -37939,7 +37939,7 @@
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.71"/>

</xml_diff>